<commit_message>
Cod pentru setul de teste minimale
</commit_message>
<xml_diff>
--- a/proiect/ProiectFDBargaoanuBogdan.xlsx
+++ b/proiect/ProiectFDBargaoanuBogdan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\facultate\fiabilitate si diagnoza\fiabilitate-si-diagnoza\proiect\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0558CDD3-4A30-4D2A-97C7-79BE3B3ABFE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{423EFC1D-CFEE-4CD1-BF8D-8833B13E9CFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{6C0A6615-6D33-0742-B44C-E9D15E73AFBA}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{6C0A6615-6D33-0742-B44C-E9D15E73AFBA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -310,23 +310,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>295275</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>99</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>25</xdr:col>
-      <xdr:colOff>762000</xdr:colOff>
+      <xdr:colOff>790575</xdr:colOff>
       <xdr:row>150</xdr:row>
-      <xdr:rowOff>190500</xdr:rowOff>
+      <xdr:rowOff>85725</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Picture 3">
+        <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4C4F6D6F-F824-C575-D90B-DC9CE8E8EA92}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{05227E84-2839-7763-67C2-A3AD6E4DD261}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -349,7 +349,7 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="295275" y="19907250"/>
+          <a:off x="323850" y="19802475"/>
           <a:ext cx="18288000" cy="10287000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -777,8 +777,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C7A6697-571A-0F4E-A918-DE0FC93C2A5E}">
   <dimension ref="A1:AI99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="L75" sqref="L75"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="Q79" sqref="Q79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -5888,103 +5888,103 @@
       </c>
     </row>
     <row r="56" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A56" s="1">
-        <v>0</v>
-      </c>
-      <c r="B56" s="1">
-        <v>1</v>
-      </c>
-      <c r="C56" s="1">
-        <v>1</v>
-      </c>
-      <c r="D56" s="1">
-        <v>1</v>
-      </c>
-      <c r="E56" s="1">
-        <v>1</v>
-      </c>
-      <c r="F56" s="1">
-        <v>0</v>
-      </c>
-      <c r="G56">
-        <v>0</v>
-      </c>
-      <c r="H56">
-        <v>0</v>
-      </c>
-      <c r="I56">
-        <v>0</v>
-      </c>
-      <c r="J56">
-        <v>0</v>
-      </c>
-      <c r="K56">
-        <v>0</v>
-      </c>
-      <c r="L56">
-        <v>0</v>
-      </c>
-      <c r="M56">
-        <v>0</v>
-      </c>
-      <c r="N56">
-        <v>0</v>
-      </c>
-      <c r="O56">
-        <v>0</v>
-      </c>
-      <c r="P56">
-        <v>0</v>
-      </c>
-      <c r="Q56">
-        <v>0</v>
-      </c>
-      <c r="R56">
-        <v>0</v>
-      </c>
-      <c r="S56">
+      <c r="A56" s="2">
+        <v>0</v>
+      </c>
+      <c r="B56" s="2">
+        <v>1</v>
+      </c>
+      <c r="C56" s="2">
+        <v>1</v>
+      </c>
+      <c r="D56" s="2">
+        <v>1</v>
+      </c>
+      <c r="E56" s="2">
+        <v>1</v>
+      </c>
+      <c r="F56" s="2">
+        <v>0</v>
+      </c>
+      <c r="G56" s="2">
+        <v>0</v>
+      </c>
+      <c r="H56" s="2">
+        <v>0</v>
+      </c>
+      <c r="I56" s="2">
+        <v>0</v>
+      </c>
+      <c r="J56" s="2">
+        <v>0</v>
+      </c>
+      <c r="K56" s="2">
+        <v>0</v>
+      </c>
+      <c r="L56" s="2">
+        <v>0</v>
+      </c>
+      <c r="M56" s="2">
+        <v>0</v>
+      </c>
+      <c r="N56" s="2">
+        <v>0</v>
+      </c>
+      <c r="O56" s="2">
+        <v>0</v>
+      </c>
+      <c r="P56" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q56" s="2">
+        <v>0</v>
+      </c>
+      <c r="R56" s="2">
+        <v>0</v>
+      </c>
+      <c r="S56" s="2">
         <v>0</v>
       </c>
       <c r="T56" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="U56">
-        <v>0</v>
-      </c>
-      <c r="V56">
-        <v>0</v>
-      </c>
-      <c r="W56">
-        <v>0</v>
-      </c>
-      <c r="X56">
-        <v>0</v>
-      </c>
-      <c r="Y56">
-        <v>0</v>
-      </c>
-      <c r="Z56">
-        <v>0</v>
-      </c>
-      <c r="AA56">
-        <v>0</v>
-      </c>
-      <c r="AB56">
-        <v>0</v>
-      </c>
-      <c r="AC56">
-        <v>0</v>
-      </c>
-      <c r="AD56">
-        <v>0</v>
-      </c>
-      <c r="AE56">
-        <v>0</v>
-      </c>
-      <c r="AF56">
-        <v>0</v>
-      </c>
-      <c r="AG56">
+      <c r="U56" s="2">
+        <v>0</v>
+      </c>
+      <c r="V56" s="2">
+        <v>0</v>
+      </c>
+      <c r="W56" s="2">
+        <v>0</v>
+      </c>
+      <c r="X56" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y56" s="2">
+        <v>0</v>
+      </c>
+      <c r="Z56" s="2">
+        <v>0</v>
+      </c>
+      <c r="AA56" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB56" s="2">
+        <v>0</v>
+      </c>
+      <c r="AC56" s="2">
+        <v>0</v>
+      </c>
+      <c r="AD56" s="2">
+        <v>0</v>
+      </c>
+      <c r="AE56" s="2">
+        <v>0</v>
+      </c>
+      <c r="AF56" s="2">
+        <v>0</v>
+      </c>
+      <c r="AG56" s="2">
         <v>0</v>
       </c>
       <c r="AH56" s="3" t="s">

</xml_diff>